<commit_message>
stu / function upload except foreign_stu
</commit_message>
<xml_diff>
--- a/public/Excel_example/stu/stu_foreign_research.xlsx
+++ b/public/Excel_example/stu/stu_foreign_research.xlsx
@@ -37,7 +37,7 @@
     <t>備註</t>
   </si>
   <si>
-    <t>會議名稱</t>
+    <t>前往國家</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -390,7 +390,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>